<commit_message>
refactored a bit, addded some plots, added metrics to Q learning
</commit_message>
<xml_diff>
--- a/default_settings.xlsx
+++ b/default_settings.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/ncook3_gatech_edu/Documents/2019-01-CS7641/HW/04-Markov-Decision-Processes/hw4-ncook-solution/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/cs7641/tjweldon_assignment4/hw4-ncook-solution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{8AA786B7-33EC-42CE-A9FE-DF30B3FD8A4C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{50B7BF7A-CF71-4284-810D-9756718D24C3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D867FBE0-F03F-2C49-B0D4-CC263DF133F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -436,129 +437,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD10"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="19" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-500</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>-0.1</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1E-8</v>
+      </c>
+      <c r="I2">
+        <v>0.8</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0.8</v>
+      </c>
+      <c r="M2">
+        <v>0.95</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-500</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>-0.1</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="E3">
+        <v>0.8</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1E-8</v>
+      </c>
+      <c r="I3">
+        <v>0.8</v>
+      </c>
+      <c r="J3">
+        <v>1000</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0.8</v>
+      </c>
+      <c r="M3">
+        <v>0.95</v>
+      </c>
+      <c r="N3">
+        <v>1000</v>
+      </c>
+      <c r="O3">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>-1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>-0.2</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>0.8</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1E-8</v>
-      </c>
-      <c r="J2">
-        <v>0.8</v>
-      </c>
-      <c r="K2">
-        <v>10000</v>
-      </c>
-      <c r="L2">
-        <v>0.1</v>
-      </c>
-      <c r="M2">
-        <v>0.8</v>
-      </c>
-      <c r="N2">
-        <v>0.95</v>
-      </c>
-      <c r="O2">
-        <v>10000</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b">
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished paper and all experiements
</commit_message>
<xml_diff>
--- a/default_settings.xlsx
+++ b/default_settings.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/cs7641/tjweldon_assignment4/hw4-ncook-solution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096F2A30-CA42-FF4A-ABFA-9BE7D8D305F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D41C29-DF2F-5D45-BDA5-B024D9761C31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25580" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>rH</t>
   </si>
@@ -78,13 +77,16 @@
   </si>
   <si>
     <t>enabled</t>
+  </si>
+  <si>
+    <t>run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,7 +97,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,11 +140,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,195 +450,491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" customWidth="1"/>
-    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:20">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
         <v>-1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>-0.1</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="3">
         <v>4</v>
       </c>
-      <c r="E2">
-        <v>0.8</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.8</v>
-      </c>
-      <c r="J2">
+      <c r="F2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1E-8</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="3">
         <v>100</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0.8</v>
-      </c>
-      <c r="M2">
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="N2" s="3">
         <v>0.95</v>
       </c>
-      <c r="N2">
+      <c r="O2" s="3">
         <v>250</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b">
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>-100</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:20">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1E-8</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="3">
         <v>100</v>
       </c>
-      <c r="C3">
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O3" s="3">
+        <v>250</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
         <v>-0.1</v>
       </c>
-      <c r="D3">
+      <c r="E4" s="3">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1E-8</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="K4" s="3">
+        <v>100</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O4" s="3">
+        <v>500</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>500</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="E5" s="3">
         <v>20</v>
       </c>
-      <c r="E3">
-        <v>0.8</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0.8</v>
-      </c>
-      <c r="J3">
+      <c r="F5" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1E-8</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5000</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1E-8</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>500</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1E-8</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="3">
         <v>100</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0.8</v>
-      </c>
-      <c r="M3">
-        <v>0.95</v>
-      </c>
-      <c r="N3">
-        <v>250</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S3" t="b">
-        <v>1</v>
-      </c>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="O7" s="3">
+        <v>500</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>